<commit_message>
Rescoring free recall data w/ multi
formatting the data for sens/spef was a hoot. But it works!
</commit_message>
<xml_diff>
--- a/Free Recall/NEW/4 Scored Datasets/Huff et al Key.xlsx
+++ b/Free Recall/NEW/4 Scored Datasets/Huff et al Key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\lrd\free_recall_SHINY\Test Data RGN\lrd paper Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickm.000\Documents\GitHub\lrd-analysis\Free Recall\NEW\4 Scored Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAE15FC-2E2D-48BC-A21B-B4EC29B539B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF32EF9-CC17-4B29-A2A9-BA7E4347F681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" activeTab="5" xr2:uid="{0C69F891-69EB-4909-88C8-1D79C299BE10}"/>
+    <workbookView xWindow="16200" yWindow="3360" windowWidth="20460" windowHeight="10950" xr2:uid="{0C69F891-69EB-4909-88C8-1D79C299BE10}"/>
   </bookViews>
   <sheets>
     <sheet name="Version A" sheetId="1" r:id="rId1"/>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC29764-7A87-425E-93DB-BB69BC9DA1AC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1579,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B7BA29-CCA9-4354-943B-C2CB23D4D86D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2884,7 +2884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB609F0A-F366-4053-BC67-AA8074D5C9B5}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
@@ -3319,11 +3319,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9DB326-D015-4925-8A13-775CCA609628}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>